<commit_message>
On branch master Changes to be committed: 	modified:   planes.xlsx 	new file:   requerimientos.doc 	modified:   tspi/ciclo-1/forma-logt1-20106065.xlsx 	modified:   tspi/plantillas/forma-logt.xlsx
</commit_message>
<xml_diff>
--- a/planes.xlsx
+++ b/planes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Totales" sheetId="1" state="visible" r:id="rId2"/>
@@ -521,7 +521,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -603,16 +603,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.178423236514523</c:v>
+                  <c:v>0.175</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.402489626556017</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.684647302904564</c:v>
+                  <c:v>0.683333333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.908713692946058</c:v>
+                  <c:v>0.908333333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -713,48 +713,48 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.029045643153527</c:v>
+                  <c:v>0.0291666666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.029045643153527</c:v>
+                  <c:v>0.0291666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.029045643153527</c:v>
+                  <c:v>0.0291666666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.029045643153527</c:v>
+                  <c:v>0.0291666666666667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.029045643153527</c:v>
+                  <c:v>0.0291666666666667</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.029045643153527</c:v>
+                  <c:v>0.0291666666666667</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.029045643153527</c:v>
+                  <c:v>0.0291666666666667</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.029045643153527</c:v>
+                  <c:v>0.0291666666666667</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.029045643153527</c:v>
+                  <c:v>0.0291666666666667</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.029045643153527</c:v>
+                  <c:v>0.0291666666666667</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.029045643153527</c:v>
+                  <c:v>0.0291666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="95167471"/>
-        <c:axId val="82585337"/>
+        <c:axId val="96612585"/>
+        <c:axId val="56706524"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95167471"/>
+        <c:axId val="96612585"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -762,7 +762,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82585337"/>
+        <c:crossAx val="56706524"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -776,7 +776,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82585337"/>
+        <c:axId val="56706524"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -793,7 +793,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95167471"/>
+        <c:crossAx val="96612585"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -830,15 +830,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:colOff>116280</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>42480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>236160</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>51480</xdr:rowOff>
+      <xdr:colOff>352080</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>11160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -846,8 +846,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="2754360"/>
-        <a:ext cx="8112600" cy="3715560"/>
+        <a:off x="116280" y="2619000"/>
+        <a:ext cx="8116560" cy="3461400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -872,8 +872,8 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.7764705882353"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="2" width="8.40392156862745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.7960784313725"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="2" width="8.41176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
@@ -891,7 +891,7 @@
       </c>
       <c r="B2" s="2" t="n">
         <f aca="false">SUM(Proyecto!E2:E198)</f>
-        <v>120.5</v>
+        <v>120</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="3">
@@ -934,21 +934,21 @@
   </sheetPr>
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B29" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G39" activeCellId="0" pane="topLeft" sqref="G39"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="G5" activeCellId="0" pane="topLeft" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="5" width="3.01960784313725"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="37.2823529411765"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="27.8"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="27.8078431372549"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.8470588235294"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="12.8549019607843"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="12.8549019607843"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="12.8549019607843"/>
-    <col collapsed="false" hidden="false" max="1021" min="9" style="2" width="8.40392156862745"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.40392156862745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="37.3098039215686"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="27.8156862745098"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="27.8274509803922"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.8549019607843"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="12.8588235294118"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="12.8588235294118"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="12.8588235294118"/>
+    <col collapsed="false" hidden="false" max="1021" min="9" style="2" width="8.41176470588235"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.41176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="1" s="10">
@@ -992,7 +992,7 @@
       </c>
       <c r="F2" s="4" t="n">
         <f aca="false">E2/_vTDHE</f>
-        <v>0.004149377593361</v>
+        <v>0.00416666666666667</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>1</v>
@@ -1019,7 +1019,7 @@
       </c>
       <c r="F3" s="4" t="n">
         <f aca="false">E3/_vTDHE</f>
-        <v>0.004149377593361</v>
+        <v>0.00416666666666667</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>1</v>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="F4" s="4" t="n">
         <f aca="false">E4/_vTDHE</f>
-        <v>0.004149377593361</v>
+        <v>0.00416666666666667</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>1</v>
@@ -1073,7 +1073,7 @@
       </c>
       <c r="F5" s="4" t="n">
         <f aca="false">E5/_vTDHE</f>
-        <v>0.016597510373444</v>
+        <v>0.0166666666666667</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>1</v>
@@ -1096,11 +1096,11 @@
         <v>21</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="F6" s="4" t="n">
         <f aca="false">E6/_vTDHE</f>
-        <v>0.020746887966805</v>
+        <v>0.0166666666666667</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>1</v>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="F7" s="4" t="n">
         <f aca="false">E7/_vTDHE</f>
-        <v>0.0829875518672199</v>
+        <v>0.0833333333333333</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>1</v>
@@ -1142,7 +1142,7 @@
       </c>
       <c r="F8" s="4" t="n">
         <f aca="false">E8/_vTDHE</f>
-        <v>0.024896265560166</v>
+        <v>0.025</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>1</v>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="F9" s="4" t="n">
         <f aca="false">E9/_vTDHE</f>
-        <v>0.004149377593361</v>
+        <v>0.00416666666666667</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>1</v>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="F10" s="4" t="n">
         <f aca="false">E10/_vTDHE</f>
-        <v>0.016597510373444</v>
+        <v>0.0166666666666667</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>1</v>
@@ -1205,7 +1205,7 @@
       </c>
       <c r="F11" s="4" t="n">
         <f aca="false">E11/_vTDHE</f>
-        <v>0.0829875518672199</v>
+        <v>0.0833333333333333</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>2</v>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="F12" s="4" t="n">
         <f aca="false">E12/_vTDHE</f>
-        <v>0.024896265560166</v>
+        <v>0.025</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>2</v>
@@ -1247,7 +1247,7 @@
       </c>
       <c r="F13" s="4" t="n">
         <f aca="false">E13/_vTDHE</f>
-        <v>0.004149377593361</v>
+        <v>0.00416666666666667</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>2</v>
@@ -1268,7 +1268,7 @@
       </c>
       <c r="F14" s="4" t="n">
         <f aca="false">E14/_vTDHE</f>
-        <v>0.016597510373444</v>
+        <v>0.0166666666666667</v>
       </c>
       <c r="G14" s="2" t="n">
         <v>2</v>
@@ -1289,7 +1289,7 @@
       </c>
       <c r="F15" s="4" t="n">
         <f aca="false">E15/_vTDHE</f>
-        <v>0.0497925311203319</v>
+        <v>0.05</v>
       </c>
       <c r="G15" s="2" t="n">
         <v>2</v>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="F16" s="4" t="n">
         <f aca="false">E16/_vTDHE</f>
-        <v>0.024896265560166</v>
+        <v>0.025</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>2</v>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="F17" s="4" t="n">
         <f aca="false">E17/_vTDHE</f>
-        <v>0.004149377593361</v>
+        <v>0.00416666666666667</v>
       </c>
       <c r="G17" s="2" t="n">
         <v>2</v>
@@ -1352,7 +1352,7 @@
       </c>
       <c r="F18" s="4" t="n">
         <f aca="false">E18/_vTDHE</f>
-        <v>0.016597510373444</v>
+        <v>0.0166666666666667</v>
       </c>
       <c r="G18" s="2" t="n">
         <v>2</v>
@@ -1373,7 +1373,7 @@
       </c>
       <c r="F19" s="4" t="n">
         <f aca="false">E19/_vTDHE</f>
-        <v>0.020746887966805</v>
+        <v>0.0208333333333333</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>3</v>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="F20" s="4" t="n">
         <f aca="false">E20/_vTDHE</f>
-        <v>0.024896265560166</v>
+        <v>0.025</v>
       </c>
       <c r="G20" s="2" t="n">
         <v>3</v>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="F21" s="4" t="n">
         <f aca="false">E21/_vTDHE</f>
-        <v>0.04149377593361</v>
+        <v>0.0416666666666667</v>
       </c>
       <c r="G21" s="2" t="n">
         <v>3</v>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="F22" s="4" t="n">
         <f aca="false">E22/_vTDHE</f>
-        <v>0.0829875518672199</v>
+        <v>0.0833333333333333</v>
       </c>
       <c r="G22" s="2" t="n">
         <v>3</v>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="F23" s="4" t="n">
         <f aca="false">E23/_vTDHE</f>
-        <v>0.04149377593361</v>
+        <v>0.0416666666666667</v>
       </c>
       <c r="G23" s="2" t="n">
         <v>3</v>
@@ -1478,7 +1478,7 @@
       </c>
       <c r="F24" s="4" t="n">
         <f aca="false">E24/_vTDHE</f>
-        <v>0.024896265560166</v>
+        <v>0.025</v>
       </c>
       <c r="G24" s="2" t="n">
         <v>3</v>
@@ -1499,7 +1499,7 @@
       </c>
       <c r="F25" s="4" t="n">
         <f aca="false">E25/_vTDHE</f>
-        <v>0.024896265560166</v>
+        <v>0.025</v>
       </c>
       <c r="G25" s="2" t="n">
         <v>3</v>
@@ -1520,7 +1520,7 @@
       </c>
       <c r="F26" s="4" t="n">
         <f aca="false">E26/_vTDHE</f>
-        <v>0.004149377593361</v>
+        <v>0.00416666666666667</v>
       </c>
       <c r="G26" s="2" t="n">
         <v>3</v>
@@ -1541,7 +1541,7 @@
       </c>
       <c r="F27" s="4" t="n">
         <f aca="false">E27/_vTDHE</f>
-        <v>0.016597510373444</v>
+        <v>0.0166666666666667</v>
       </c>
       <c r="G27" s="2" t="n">
         <v>3</v>
@@ -1562,7 +1562,7 @@
       </c>
       <c r="F28" s="4" t="n">
         <f aca="false">E28/_vTDHE</f>
-        <v>0.0829875518672199</v>
+        <v>0.0833333333333333</v>
       </c>
       <c r="G28" s="2" t="n">
         <v>4</v>
@@ -1583,7 +1583,7 @@
       </c>
       <c r="F29" s="4" t="n">
         <f aca="false">E29/_vTDHE</f>
-        <v>0.024896265560166</v>
+        <v>0.025</v>
       </c>
       <c r="G29" s="2" t="n">
         <v>4</v>
@@ -1604,7 +1604,7 @@
       </c>
       <c r="F30" s="4" t="n">
         <f aca="false">E30/_vTDHE</f>
-        <v>0.004149377593361</v>
+        <v>0.00416666666666667</v>
       </c>
       <c r="G30" s="2" t="n">
         <v>4</v>
@@ -1625,7 +1625,7 @@
       </c>
       <c r="F31" s="4" t="n">
         <f aca="false">E31/_vTDHE</f>
-        <v>0.016597510373444</v>
+        <v>0.0166666666666667</v>
       </c>
       <c r="G31" s="2" t="n">
         <v>4</v>
@@ -1646,7 +1646,7 @@
       </c>
       <c r="F32" s="4" t="n">
         <f aca="false">E32/_vTDHE</f>
-        <v>0.0497925311203319</v>
+        <v>0.05</v>
       </c>
       <c r="G32" s="2" t="n">
         <v>4</v>
@@ -1667,7 +1667,7 @@
       </c>
       <c r="F33" s="4" t="n">
         <f aca="false">E33/_vTDHE</f>
-        <v>0.024896265560166</v>
+        <v>0.025</v>
       </c>
       <c r="G33" s="2" t="n">
         <v>4</v>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="F34" s="4" t="n">
         <f aca="false">E34/_vTDHE</f>
-        <v>0.004149377593361</v>
+        <v>0.00416666666666667</v>
       </c>
       <c r="G34" s="2" t="n">
         <v>4</v>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="F35" s="4" t="n">
         <f aca="false">E35/_vTDHE</f>
-        <v>0.016597510373444</v>
+        <v>0.0166666666666667</v>
       </c>
       <c r="G35" s="2" t="n">
         <v>4</v>
@@ -1730,7 +1730,7 @@
       </c>
       <c r="F36" s="4" t="n">
         <f aca="false">E36/_vTDHE</f>
-        <v>0.024896265560166</v>
+        <v>0.025</v>
       </c>
       <c r="G36" s="2" t="n">
         <v>5</v>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="F37" s="4" t="n">
         <f aca="false">E37/_vTDHE</f>
-        <v>0.024896265560166</v>
+        <v>0.025</v>
       </c>
       <c r="G37" s="2" t="n">
         <v>5</v>
@@ -1772,7 +1772,7 @@
       </c>
       <c r="F38" s="4" t="n">
         <f aca="false">E38/_vTDHE</f>
-        <v>0.04149377593361</v>
+        <v>0.0416666666666667</v>
       </c>
       <c r="G38" s="2" t="n">
         <v>5</v>
@@ -1796,13 +1796,13 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D5" activeCellId="0" pane="topLeft" sqref="D5"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="2" width="11.6274509803922"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="2" width="10.5725490196078"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="2" width="11.6352941176471"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="2" width="10.5764705882353"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="51.65" outlineLevel="0" r="1" s="10">
@@ -1843,11 +1843,11 @@
       </c>
       <c r="D2" s="11" t="n">
         <f aca="false">SUMIF(_cS, A2, _cHE)</f>
-        <v>21.5</v>
+        <v>21</v>
       </c>
       <c r="E2" s="13" t="n">
         <f aca="false">SUMIF(_cS, A2, _cPIDHE)</f>
-        <v>0.178423236514523</v>
+        <v>0.175</v>
       </c>
       <c r="F2" s="13" t="inlineStr">
         <f aca="false">E2</f>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="G2" s="13" t="n">
         <f aca="false">SUMIF(_cS, A2, _cPIDHO)</f>
-        <v>0.029045643153527</v>
+        <v>0.0291666666666667</v>
       </c>
       <c r="H2" s="13" t="inlineStr">
         <f aca="false">G2</f>
@@ -1885,7 +1885,7 @@
       </c>
       <c r="E3" s="13" t="n">
         <f aca="false">SUMIF(_cS, A3, _cPIDHE)</f>
-        <v>0.224066390041494</v>
+        <v>0.225</v>
       </c>
       <c r="F3" s="13" t="inlineStr">
         <f aca="false">E3+F2</f>
@@ -1923,7 +1923,7 @@
       </c>
       <c r="E4" s="13" t="n">
         <f aca="false">SUMIF(_cS, A4, _cPIDHE)</f>
-        <v>0.282157676348548</v>
+        <v>0.283333333333333</v>
       </c>
       <c r="F4" s="13" t="inlineStr">
         <f aca="false">E4+F3</f>
@@ -1961,7 +1961,7 @@
       </c>
       <c r="E5" s="13" t="n">
         <f aca="false">SUMIF(_cS, A5, _cPIDHE)</f>
-        <v>0.224066390041494</v>
+        <v>0.225</v>
       </c>
       <c r="F5" s="13" t="inlineStr">
         <f aca="false">E5+F4</f>
@@ -1999,7 +1999,7 @@
       </c>
       <c r="E6" s="13" t="n">
         <f aca="false">SUMIF(_cS, A6, _cPIDHE)</f>
-        <v>0.0912863070539419</v>
+        <v>0.0916666666666667</v>
       </c>
       <c r="F6" s="13" t="inlineStr">
         <f aca="false">E6+F5</f>

</xml_diff>

<commit_message>
On branch master Changes to be committed: 	modified:   planes.xlsx 	modified:   requerimientos.doc 	modified:   tspi/ciclo-1/forma-logt1-20106065.xlsx
</commit_message>
<xml_diff>
--- a/planes.xlsx
+++ b/planes.xlsx
@@ -5,18 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="3" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="456" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Totales" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Proyecto" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Recursos" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Ciclo1" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="_cHE" vbProcedure="false">Proyecto!$E$2:$E$1048576</definedName>
-    <definedName function="false" hidden="false" name="_cPIDHE" vbProcedure="false">Proyecto!$F$2:$F$1048573</definedName>
-    <definedName function="false" hidden="false" name="_cPIDHO" vbProcedure="false">Proyecto!$H$2:$H$1048573</definedName>
-    <definedName function="false" hidden="false" name="_cS" vbProcedure="false">Proyecto!$G$2:$G$1048573</definedName>
+    <definedName function="false" hidden="false" name="_cHE" vbProcedure="false">Proyecto!$F$2:$F$1048576</definedName>
+    <definedName function="false" hidden="false" name="_cPIDHE" vbProcedure="false">Proyecto!$G$2:$G$1048576</definedName>
+    <definedName function="false" hidden="false" name="_cPIDHO" vbProcedure="false">Proyecto!$I$2:$I$1048576</definedName>
+    <definedName function="false" hidden="false" name="_cS" vbProcedure="false">Proyecto!$H$2:$H$1048576</definedName>
     <definedName function="false" hidden="false" name="_vPTDGO" vbProcedure="false">Totales!$B$6</definedName>
     <definedName function="false" hidden="false" name="_vTDD" vbProcedure="false">Totales!$B$1</definedName>
     <definedName function="false" hidden="false" name="_vTDHE" vbProcedure="false">Totales!$B$2</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="139">
   <si>
     <t>Total de Horas Disponibles</t>
   </si>
@@ -47,6 +48,9 @@
     <t>Tarea</t>
   </si>
   <si>
+    <t>Padre</t>
+  </si>
+  <si>
     <t>Criterio de Entrada</t>
   </si>
   <si>
@@ -83,9 +87,15 @@
     <t>Agenda para la reunion #1 con el cliente.</t>
   </si>
   <si>
+    <t>Experimiento RedMine #1</t>
+  </si>
+  <si>
     <t>Reunión #1 con el cliente.</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>Minuta de la reunión #1 con el cliente.</t>
   </si>
   <si>
@@ -98,72 +108,114 @@
     <t>Analizar los requerimientos obtenidos en la reunión #1.</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>Borrador #1 de los casos de uso; Borrador #1 de los escenarios.</t>
   </si>
   <si>
     <t>Crear el borrador #1 del documento de requerimientos.</t>
   </si>
   <si>
+    <t>6; 7</t>
+  </si>
+  <si>
     <t>Borrador #1 del documento de requerimientos.</t>
   </si>
   <si>
     <t>Crear la agenda para la reunión #2 con el cliente.</t>
   </si>
   <si>
+    <t>8</t>
+  </si>
+  <si>
     <t>Agenda para la reunion #2 con el cliente.</t>
   </si>
   <si>
     <t>Reunión #2 con el cliente.</t>
   </si>
   <si>
+    <t>9</t>
+  </si>
+  <si>
     <t>Minuta de la reunión #2 con el cliente.</t>
   </si>
   <si>
     <t>Analizar los requerimientos obtenidos en la reunión #2, y actualizar los borradores de los casos de uso y escenarios.</t>
   </si>
   <si>
+    <t>10</t>
+  </si>
+  <si>
     <t>Borrador #2 de los casos de uso; Borrador #2 de los escenarios.</t>
   </si>
   <si>
+    <t>Experimiento Ruby #1</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>Actualizar el borrador #1 del documento de requerimientos.</t>
   </si>
   <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>Borrador #2 del documento de requerimientos.</t>
   </si>
   <si>
     <t>Crear la agenda para la reunión #3 con el cliente.</t>
   </si>
   <si>
+    <t>13</t>
+  </si>
+  <si>
     <t>Agenda para la reunion #3 con el cliente.</t>
   </si>
   <si>
     <t>Reunión #3 con el cliente.</t>
   </si>
   <si>
+    <t>14</t>
+  </si>
+  <si>
     <t>Minuta de la reunión #3 con el cliente.</t>
   </si>
   <si>
     <t>Analizar los requerimientos obtenidos en la reunión #3 y actualizar los borradores de los casos de uso y escenarios.</t>
   </si>
   <si>
+    <t>15</t>
+  </si>
+  <si>
     <t>Borrador #3 de los casos de uso; Borrador #3 de los escenarios.</t>
   </si>
   <si>
     <t>Crear la versión final del documento de requerimientos.</t>
   </si>
   <si>
+    <t>16</t>
+  </si>
+  <si>
     <t>Versión final del documento de requerimientos.</t>
   </si>
   <si>
     <t>Crear la agenda para la reunión #4 con el cliente.</t>
   </si>
   <si>
+    <t>17</t>
+  </si>
+  <si>
     <t>Agenda para la reunion #4 con el cliente.</t>
   </si>
   <si>
     <t>Reunión #4 con el cliente.</t>
   </si>
   <si>
+    <t>18</t>
+  </si>
+  <si>
     <t>Minuta de la reunión #4 con el cliente.</t>
   </si>
   <si>
@@ -182,12 +234,18 @@
     <t>Definir las tácticas y patrones a utilizar.</t>
   </si>
   <si>
+    <t>21</t>
+  </si>
+  <si>
     <t>Borrador #1 de las especificaciones de las tácticas y patrones a utilizar.</t>
   </si>
   <si>
     <t>Crear el borrador #1 de la vista estática de la arquitectura.</t>
   </si>
   <si>
+    <t>22</t>
+  </si>
+  <si>
     <t>Borrador #1 de la vista estática de la arquitectura.</t>
   </si>
   <si>
@@ -206,66 +264,105 @@
     <t>Crear el borrador #1 del documento de la arquitectura.</t>
   </si>
   <si>
+    <t>20; 21; 22; 23; 24; 25</t>
+  </si>
+  <si>
     <t>Borrador #1 del documento de la arquitectura.</t>
   </si>
   <si>
     <t>Crear la agenda para la reunión #5 con el cliente.</t>
   </si>
   <si>
+    <t>26</t>
+  </si>
+  <si>
     <t>Agenda para la reunion #5 con el cliente.</t>
   </si>
   <si>
     <t>Reunión #5 con el cliente.</t>
   </si>
   <si>
+    <t>27</t>
+  </si>
+  <si>
     <t>Minuta de la reunión #5 con el cliente.</t>
   </si>
   <si>
     <t>Analizar los comentarios de la reunión #5, y actualizar el borrador del diagrama de contexto, la especificación de las tácticas y patrones, y los borradores de las vistas de la arquitectura.</t>
   </si>
   <si>
+    <t>28</t>
+  </si>
+  <si>
     <t>Borrador #2 del diagrama de contexto; Borrador #2 de la especificación de las tácticas y patrones a utilizar; Borrador #2 de la vista estática, dinámica y física de la arquitectura;</t>
   </si>
   <si>
     <t>Crear el borrador #2 del documento de la arquitectura.</t>
   </si>
   <si>
+    <t>29</t>
+  </si>
+  <si>
     <t>Borrador #2 del documento de la arquitectura.</t>
   </si>
   <si>
     <t>Crear la agenda para la reunión #6 con el cliente.</t>
   </si>
   <si>
+    <t>30</t>
+  </si>
+  <si>
     <t>Agenda para la reunion #6 con el cliente.</t>
   </si>
   <si>
     <t>Reunión #6 con el cliente.</t>
   </si>
   <si>
+    <t>31</t>
+  </si>
+  <si>
     <t>Minuta de la reunión #6 con el cliente.</t>
   </si>
   <si>
     <t>Analizar los comentarios de la reunión #6, y actualizar el borrador del diagrama de contexto, la especificación de las tácticas y patrones, y los borradores de las vistas de la arquitectura.</t>
   </si>
   <si>
+    <t>32</t>
+  </si>
+  <si>
     <t>Borrador #3 del diagrama de contexto; Borrador #3 de la especificación de las tácticas y patrones a utilizar; Borrador #3 de la vista estática, dinámica y física de la arquitectura;</t>
   </si>
   <si>
     <t>Crear la versión final del documento de la arquitectura.</t>
   </si>
   <si>
+    <t>33</t>
+  </si>
+  <si>
     <t>Versión final del documento de la arquitectura.</t>
   </si>
   <si>
+    <t>Experimiento Ruby #2</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
     <t>Crear la agenda para la reunión #7 con el cliente.</t>
   </si>
   <si>
+    <t>34</t>
+  </si>
+  <si>
     <t>Agenda para la reunion #7 con el cliente.</t>
   </si>
   <si>
     <t>Reunión #7 con el cliente.</t>
   </si>
   <si>
+    <t>36</t>
+  </si>
+  <si>
     <t>Minuta de la reunión #7 con el cliente.</t>
   </si>
   <si>
@@ -278,15 +375,30 @@
     <t>Construir el documento a presentar en la presentación #1 del curso.</t>
   </si>
   <si>
+    <t>19; 37</t>
+  </si>
+  <si>
     <t>Documento de la presentación media del curso.</t>
   </si>
   <si>
     <t>Presentación #1 del curso.</t>
   </si>
   <si>
+    <t>39</t>
+  </si>
+  <si>
     <t>Minuta de la presentación #1 del curso.</t>
   </si>
   <si>
+    <t>Experimiento MySQL #1</t>
+  </si>
+  <si>
+    <t>Experimiento Ruby #3</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
     <t>Fecha de inicio</t>
   </si>
   <si>
@@ -303,16 +415,48 @@
   </si>
   <si>
     <t>Porcentaje de las Ganacias Obtenidas</t>
+  </si>
+  <si>
+    <t>3 Semanas; 09/16/2014-10/06/2014</t>
+  </si>
+  <si>
+    <t>Asignado a</t>
+  </si>
+  <si>
+    <t>Fecha Estimada de Inicio</t>
+  </si>
+  <si>
+    <t>Fecha de Inicio</t>
+  </si>
+  <si>
+    <t>Fecha Estimada de Finalización</t>
+  </si>
+  <si>
+    <t>Fecha de Finalización</t>
+  </si>
+  <si>
+    <t>Horas Trabajadas</t>
+  </si>
+  <si>
+    <t>HVR</t>
+  </si>
+  <si>
+    <t>HVR; JGR; JV; AA; GW</t>
+  </si>
+  <si>
+    <t>HVR; AA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="0.00%" numFmtId="165"/>
-    <numFmt formatCode="MM/DD/YY" numFmtId="166"/>
+    <numFmt formatCode="@" numFmtId="166"/>
+    <numFmt formatCode="MM/DD/YY" numFmtId="167"/>
+    <numFmt formatCode="MM/DD/YYYY" numFmtId="168"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -420,7 +564,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
@@ -431,10 +575,13 @@
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="166" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
@@ -442,13 +589,23 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="6" numFmtId="166" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="6" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="166" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="167" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="167" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="168" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="6" numFmtId="168" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -521,7 +678,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -603,19 +760,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.175</c:v>
+                  <c:v>0.0692771084337349</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4</c:v>
+                  <c:v>0.174698795180723</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.683333333333333</c:v>
+                  <c:v>0.409638554216868</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.908333333333333</c:v>
+                  <c:v>0.614457831325301</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0.837349397590362</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -713,48 +870,48 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.0291666666666667</c:v>
+                  <c:v>0.00903614457831325</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0291666666666667</c:v>
+                  <c:v>0.0210843373493976</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0291666666666667</c:v>
+                  <c:v>0.0210843373493976</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0291666666666667</c:v>
+                  <c:v>0.0210843373493976</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0291666666666667</c:v>
+                  <c:v>0.0210843373493976</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0291666666666667</c:v>
+                  <c:v>0.0210843373493976</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0291666666666667</c:v>
+                  <c:v>0.0210843373493976</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0291666666666667</c:v>
+                  <c:v>0.0210843373493976</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0291666666666667</c:v>
+                  <c:v>0.0210843373493976</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0291666666666667</c:v>
+                  <c:v>0.0210843373493976</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0291666666666667</c:v>
+                  <c:v>0.0210843373493976</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="96612585"/>
-        <c:axId val="56706524"/>
+        <c:axId val="92389958"/>
+        <c:axId val="94794816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96612585"/>
+        <c:axId val="92389958"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -762,7 +919,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56706524"/>
+        <c:crossAx val="94794816"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -776,7 +933,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56706524"/>
+        <c:axId val="94794816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -793,7 +950,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96612585"/>
+        <c:crossAx val="92389958"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -829,16 +986,16 @@
 <xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>116280</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>42480</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>167400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>34920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>352080</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>11160</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>93960</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -846,8 +1003,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="116280" y="2619000"/>
-        <a:ext cx="8116560" cy="3461400"/>
+        <a:off x="9179280" y="34920"/>
+        <a:ext cx="8120520" cy="3219480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -868,12 +1025,12 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C9" activeCellId="0" pane="topLeft" sqref="C9"/>
+      <selection activeCell="C9" activeCellId="1" pane="topLeft" sqref="I21 C9"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.7960784313725"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="2" width="8.41176470588235"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="2" width="8.41960784313726"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
@@ -890,8 +1047,8 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <f aca="false">SUM(Proyecto!E2:E198)</f>
-        <v>120</v>
+        <f aca="false">SUM(Proyecto!F2:F201)</f>
+        <v>166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="3">
@@ -932,49 +1089,53 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G5" activeCellId="0" pane="topLeft" sqref="G5"/>
+      <selection activeCell="H20" activeCellId="1" pane="topLeft" sqref="I21 H20"/>
     </sheetView>
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="5" width="3.01960784313725"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="37.3098039215686"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="27.8156862745098"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="27.8274509803922"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="12.8549019607843"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="12.8588235294118"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="12.8588235294118"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="12.8588235294118"/>
-    <col collapsed="false" hidden="false" max="1021" min="9" style="2" width="8.41176470588235"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.41176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="37.3372549019608"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="12.5529411764706"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="27.8352941176471"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="27.8470588235294"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="12.8588235294118"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="12.8666666666667"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="12.8666666666667"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="4" width="12.8666666666667"/>
+    <col collapsed="false" hidden="false" max="1022" min="10" style="2" width="8.41960784313726"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.41960784313726"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="1" s="10">
-      <c r="A1" s="7" t="s">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="1" s="12">
+      <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="11" t="s">
         <v>10</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>11</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="2">
@@ -982,23 +1143,23 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="n">
         <v>0.5</v>
       </c>
-      <c r="F2" s="4" t="n">
-        <f aca="false">E2/_vTDHE</f>
-        <v>0.00416666666666667</v>
-      </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="4" t="n">
+        <f aca="false">F2/_vTDHE</f>
+        <v>0.00301204819277108</v>
+      </c>
+      <c r="H2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H2" s="4" t="inlineStr">
-        <f aca="false">F2</f>
+      <c r="I2" s="4" t="inlineStr">
+        <f aca="false">G2</f>
         <is>
           <t/>
         </is>
@@ -1009,23 +1170,23 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="n">
         <v>0.5</v>
       </c>
-      <c r="F3" s="4" t="n">
-        <f aca="false">E3/_vTDHE</f>
-        <v>0.00416666666666667</v>
-      </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="4" t="n">
+        <f aca="false">F3/_vTDHE</f>
+        <v>0.00301204819277108</v>
+      </c>
+      <c r="H3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H3" s="4" t="inlineStr">
-        <f aca="false">F3</f>
+      <c r="I3" s="4" t="inlineStr">
+        <f aca="false">G3</f>
         <is>
           <t/>
         </is>
@@ -1036,23 +1197,23 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2" t="n">
         <v>0.5</v>
       </c>
-      <c r="F4" s="4" t="n">
-        <f aca="false">E4/_vTDHE</f>
-        <v>0.00416666666666667</v>
-      </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="4" t="n">
+        <f aca="false">F4/_vTDHE</f>
+        <v>0.00301204819277108</v>
+      </c>
+      <c r="H4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="H4" s="4" t="inlineStr">
-        <f aca="false">F4</f>
+      <c r="I4" s="4" t="inlineStr">
+        <f aca="false">G4</f>
         <is>
           <t/>
         </is>
@@ -1063,26 +1224,17 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F5" s="4" t="n">
-        <f aca="false">E5/_vTDHE</f>
-        <v>0.0166666666666667</v>
-      </c>
-      <c r="G5" s="2" t="n">
+      <c r="F5" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <f aca="false">F5/_vTDHE</f>
+        <v>0.0602409638554217</v>
+      </c>
+      <c r="H5" s="2" t="n">
         <v>1</v>
-      </c>
-      <c r="H5" s="4" t="inlineStr">
-        <f aca="false">F5</f>
-        <is>
-          <t/>
-        </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="6">
@@ -1092,39 +1244,48 @@
       <c r="B6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="F6" s="4" t="n">
-        <f aca="false">E6/_vTDHE</f>
-        <v>0.0166666666666667</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="7">
+      <c r="G6" s="4" t="n">
+        <f aca="false">F6/_vTDHE</f>
+        <v>0.0120481927710843</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" s="4" t="inlineStr">
+        <f aca="false">G6</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="7">
       <c r="A7" s="5" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="F7" s="4" t="n">
-        <f aca="false">E7/_vTDHE</f>
-        <v>0.0833333333333333</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>1</v>
+      <c r="E7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <f aca="false">F7/_vTDHE</f>
+        <v>0.0120481927710843</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="8">
@@ -1132,41 +1293,47 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F8" s="4" t="n">
-        <f aca="false">E8/_vTDHE</f>
-        <v>0.025</v>
-      </c>
-      <c r="G8" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="9">
+      <c r="C8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G8" s="4" t="n">
+        <f aca="false">F8/_vTDHE</f>
+        <v>0.0602409638554217</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="9">
       <c r="A9" s="5" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F9" s="4" t="n">
-        <f aca="false">E9/_vTDHE</f>
-        <v>0.00416666666666667</v>
-      </c>
-      <c r="G9" s="2" t="n">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G9" s="4" t="n">
+        <f aca="false">F9/_vTDHE</f>
+        <v>0.0180722891566265</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="10">
@@ -1174,41 +1341,47 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="4" t="n">
+        <f aca="false">F10/_vTDHE</f>
+        <v>0.00301204819277108</v>
+      </c>
+      <c r="H10" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="F10" s="4" t="n">
-        <f aca="false">E10/_vTDHE</f>
-        <v>0.0166666666666667</v>
-      </c>
-      <c r="G10" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="11">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="11">
       <c r="A11" s="5" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="F11" s="4" t="n">
-        <f aca="false">E11/_vTDHE</f>
-        <v>0.0833333333333333</v>
-      </c>
-      <c r="G11" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="G11" s="4" t="n">
+        <f aca="false">F11/_vTDHE</f>
+        <v>0.0120481927710843</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>3</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="12">
@@ -1216,20 +1389,23 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F12" s="4" t="n">
-        <f aca="false">E12/_vTDHE</f>
-        <v>0.025</v>
-      </c>
-      <c r="G12" s="2" t="n">
-        <v>2</v>
+        <v>37</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G12" s="4" t="n">
+        <f aca="false">F12/_vTDHE</f>
+        <v>0.0602409638554217</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>3</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="13">
@@ -1237,125 +1413,140 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F13" s="4" t="n">
-        <f aca="false">E13/_vTDHE</f>
-        <v>0.00416666666666667</v>
-      </c>
-      <c r="G13" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="14">
+        <v>40</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G13" s="4" t="n">
+        <f aca="false">F13/_vTDHE</f>
+        <v>0.0602409638554217</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="14">
       <c r="A14" s="5" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F14" s="4" t="n">
-        <f aca="false">E14/_vTDHE</f>
-        <v>0.0166666666666667</v>
-      </c>
-      <c r="G14" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="15">
+        <v>42</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G14" s="4" t="n">
+        <f aca="false">F14/_vTDHE</f>
+        <v>0.0180722891566265</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="15">
       <c r="A15" s="5" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="F15" s="4" t="n">
-        <f aca="false">E15/_vTDHE</f>
-        <v>0.05</v>
-      </c>
-      <c r="G15" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="16">
+        <v>45</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="4" t="n">
+        <f aca="false">F15/_vTDHE</f>
+        <v>0.00301204819277108</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="16">
       <c r="A16" s="5" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F16" s="4" t="n">
-        <f aca="false">E16/_vTDHE</f>
-        <v>0.025</v>
-      </c>
-      <c r="G16" s="2" t="n">
+        <v>48</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="2" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="17">
+      <c r="G16" s="4" t="n">
+        <f aca="false">F16/_vTDHE</f>
+        <v>0.0120481927710843</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="17">
       <c r="A17" s="5" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F17" s="4" t="n">
-        <f aca="false">E17/_vTDHE</f>
-        <v>0.00416666666666667</v>
-      </c>
-      <c r="G17" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="18">
+        <v>51</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="G17" s="4" t="n">
+        <f aca="false">F17/_vTDHE</f>
+        <v>0.036144578313253</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="18">
       <c r="A18" s="5" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F18" s="4" t="n">
-        <f aca="false">E18/_vTDHE</f>
-        <v>0.0166666666666667</v>
-      </c>
-      <c r="G18" s="2" t="n">
-        <v>2</v>
+        <v>54</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G18" s="4" t="n">
+        <f aca="false">F18/_vTDHE</f>
+        <v>0.0180722891566265</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>3</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="19">
@@ -1363,19 +1554,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="2" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="F19" s="4" t="n">
-        <f aca="false">E19/_vTDHE</f>
-        <v>0.0208333333333333</v>
-      </c>
-      <c r="G19" s="2" t="n">
+        <v>57</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G19" s="4" t="n">
+        <f aca="false">F19/_vTDHE</f>
+        <v>0.00301204819277108</v>
+      </c>
+      <c r="H19" s="2" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1384,62 +1578,68 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F20" s="4" t="n">
-        <f aca="false">E20/_vTDHE</f>
-        <v>0.025</v>
-      </c>
-      <c r="G20" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="21">
+        <v>60</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G20" s="4" t="n">
+        <f aca="false">F20/_vTDHE</f>
+        <v>0.0120481927710843</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="21">
       <c r="A21" s="5" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F21" s="4" t="n">
-        <f aca="false">E21/_vTDHE</f>
-        <v>0.0416666666666667</v>
-      </c>
-      <c r="G21" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="22">
+        <v>63</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G21" s="4" t="n">
+        <f aca="false">F21/_vTDHE</f>
+        <v>0.0150602409638554</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="22">
       <c r="A22" s="5" t="n">
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="F22" s="4" t="n">
-        <f aca="false">E22/_vTDHE</f>
-        <v>0.0833333333333333</v>
-      </c>
-      <c r="G22" s="2" t="n">
-        <v>3</v>
+        <v>65</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G22" s="4" t="n">
+        <f aca="false">F22/_vTDHE</f>
+        <v>0.0180722891566265</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>4</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="23">
@@ -1447,20 +1647,23 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="2" t="n">
+        <v>67</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="F23" s="4" t="n">
-        <f aca="false">E23/_vTDHE</f>
-        <v>0.0416666666666667</v>
-      </c>
-      <c r="G23" s="2" t="n">
-        <v>3</v>
+      <c r="G23" s="4" t="n">
+        <f aca="false">F23/_vTDHE</f>
+        <v>0.0301204819277108</v>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>4</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="24">
@@ -1468,20 +1671,23 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F24" s="4" t="n">
-        <f aca="false">E24/_vTDHE</f>
-        <v>0.025</v>
-      </c>
-      <c r="G24" s="2" t="n">
-        <v>3</v>
+        <v>70</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G24" s="4" t="n">
+        <f aca="false">F24/_vTDHE</f>
+        <v>0.0602409638554217</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>4</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="25">
@@ -1489,230 +1695,263 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F25" s="4" t="n">
-        <f aca="false">E25/_vTDHE</f>
-        <v>0.025</v>
-      </c>
-      <c r="G25" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="26">
+        <v>73</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G25" s="4" t="n">
+        <f aca="false">F25/_vTDHE</f>
+        <v>0.0301204819277108</v>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="26">
       <c r="A26" s="5" t="n">
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E26" s="2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F26" s="4" t="n">
-        <f aca="false">E26/_vTDHE</f>
-        <v>0.00416666666666667</v>
-      </c>
-      <c r="G26" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="27">
+        <v>75</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G26" s="4" t="n">
+        <f aca="false">F26/_vTDHE</f>
+        <v>0.0180722891566265</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="27">
       <c r="A27" s="5" t="n">
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F27" s="4" t="n">
-        <f aca="false">E27/_vTDHE</f>
-        <v>0.0166666666666667</v>
-      </c>
-      <c r="G27" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="64.15" outlineLevel="0" r="28">
+        <v>77</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G27" s="4" t="n">
+        <f aca="false">F27/_vTDHE</f>
+        <v>0.0180722891566265</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="28">
       <c r="A28" s="5" t="n">
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="F28" s="4" t="n">
-        <f aca="false">E28/_vTDHE</f>
-        <v>0.0833333333333333</v>
-      </c>
-      <c r="G28" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G28" s="4" t="n">
+        <f aca="false">F28/_vTDHE</f>
+        <v>0.00301204819277108</v>
+      </c>
+      <c r="H28" s="2" t="n">
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="29">
       <c r="A29" s="5" t="n">
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F29" s="4" t="n">
-        <f aca="false">E29/_vTDHE</f>
-        <v>0.025</v>
-      </c>
-      <c r="G29" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G29" s="4" t="n">
+        <f aca="false">F29/_vTDHE</f>
+        <v>0.0120481927710843</v>
+      </c>
+      <c r="H29" s="2" t="n">
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="64.15" outlineLevel="0" r="30">
       <c r="A30" s="5" t="n">
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E30" s="2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F30" s="4" t="n">
-        <f aca="false">E30/_vTDHE</f>
-        <v>0.00416666666666667</v>
-      </c>
-      <c r="G30" s="2" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="31">
+        <v>86</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G30" s="4" t="n">
+        <f aca="false">F30/_vTDHE</f>
+        <v>0.0602409638554217</v>
+      </c>
+      <c r="H30" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="31">
       <c r="A31" s="5" t="n">
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E31" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F31" s="4" t="n">
-        <f aca="false">E31/_vTDHE</f>
-        <v>0.0166666666666667</v>
-      </c>
-      <c r="G31" s="2" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="64.15" outlineLevel="0" r="32">
+        <v>89</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G31" s="4" t="n">
+        <f aca="false">F31/_vTDHE</f>
+        <v>0.0180722891566265</v>
+      </c>
+      <c r="H31" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="32">
       <c r="A32" s="5" t="n">
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E32" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="F32" s="4" t="n">
-        <f aca="false">E32/_vTDHE</f>
-        <v>0.05</v>
-      </c>
-      <c r="G32" s="2" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="33">
+        <v>92</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G32" s="4" t="n">
+        <f aca="false">F32/_vTDHE</f>
+        <v>0.00301204819277108</v>
+      </c>
+      <c r="H32" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="33">
       <c r="A33" s="5" t="n">
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E33" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F33" s="4" t="n">
-        <f aca="false">E33/_vTDHE</f>
-        <v>0.025</v>
-      </c>
-      <c r="G33" s="2" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="34">
+        <v>95</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F33" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G33" s="4" t="n">
+        <f aca="false">F33/_vTDHE</f>
+        <v>0.0120481927710843</v>
+      </c>
+      <c r="H33" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="64.15" outlineLevel="0" r="34">
       <c r="A34" s="5" t="n">
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E34" s="2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F34" s="4" t="n">
-        <f aca="false">E34/_vTDHE</f>
-        <v>0.00416666666666667</v>
-      </c>
-      <c r="G34" s="2" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="35">
+        <v>98</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F34" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="G34" s="4" t="n">
+        <f aca="false">F34/_vTDHE</f>
+        <v>0.036144578313253</v>
+      </c>
+      <c r="H34" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="35">
       <c r="A35" s="5" t="n">
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E35" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F35" s="4" t="n">
-        <f aca="false">E35/_vTDHE</f>
-        <v>0.0166666666666667</v>
-      </c>
-      <c r="G35" s="2" t="n">
-        <v>4</v>
+        <v>101</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F35" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G35" s="4" t="n">
+        <f aca="false">F35/_vTDHE</f>
+        <v>0.0180722891566265</v>
+      </c>
+      <c r="H35" s="2" t="n">
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="36">
@@ -1720,40 +1959,43 @@
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E36" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F36" s="4" t="n">
-        <f aca="false">E36/_vTDHE</f>
-        <v>0.025</v>
-      </c>
-      <c r="G36" s="2" t="n">
+        <v>104</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F36" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G36" s="4" t="n">
+        <f aca="false">F36/_vTDHE</f>
+        <v>0.0602409638554217</v>
+      </c>
+      <c r="H36" s="2" t="n">
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="37">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="37">
       <c r="A37" s="5" t="n">
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E37" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F37" s="4" t="n">
-        <f aca="false">E37/_vTDHE</f>
-        <v>0.025</v>
-      </c>
-      <c r="G37" s="2" t="n">
+        <v>106</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F37" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G37" s="4" t="n">
+        <f aca="false">F37/_vTDHE</f>
+        <v>0.00301204819277108</v>
+      </c>
+      <c r="H37" s="2" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1762,20 +2004,131 @@
         <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E38" s="2" t="n">
+        <v>109</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F38" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G38" s="4" t="n">
+        <f aca="false">F38/_vTDHE</f>
+        <v>0.0120481927710843</v>
+      </c>
+      <c r="H38" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="F38" s="4" t="n">
-        <f aca="false">E38/_vTDHE</f>
-        <v>0.0416666666666667</v>
-      </c>
-      <c r="G38" s="2" t="n">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="39">
+      <c r="A39" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F39" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G39" s="4" t="n">
+        <f aca="false">F39/_vTDHE</f>
+        <v>0.0180722891566265</v>
+      </c>
+      <c r="H39" s="2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="40">
+      <c r="A40" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F40" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G40" s="4" t="n">
+        <f aca="false">F40/_vTDHE</f>
+        <v>0.0180722891566265</v>
+      </c>
+      <c r="H40" s="2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="41">
+      <c r="A41" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F41" s="2" t="n">
         <v>5</v>
+      </c>
+      <c r="G41" s="4" t="n">
+        <f aca="false">F41/_vTDHE</f>
+        <v>0.0301204819277108</v>
+      </c>
+      <c r="H41" s="2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="42">
+      <c r="A42" s="5" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F42" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="G42" s="4" t="n">
+        <f aca="false">F42/_vTDHE</f>
+        <v>0.036144578313253</v>
+      </c>
+      <c r="H42" s="2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="43">
+      <c r="A43" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F43" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G43" s="4" t="n">
+        <f aca="false">F43/_vTDHE</f>
+        <v>0.0602409638554217</v>
+      </c>
+      <c r="H43" s="2" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1794,72 +2147,72 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F7" activeCellId="1" pane="topLeft" sqref="I21 F7"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="2" width="11.6352941176471"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="2" width="10.5764705882353"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="2" width="11.6392156862745"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="2" width="10.5843137254902"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="51.65" outlineLevel="0" r="1" s="10">
-      <c r="A1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>91</v>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="51.65" outlineLevel="0" r="1" s="12">
+      <c r="A1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>128</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="2">
-      <c r="A2" s="11" t="n">
+      <c r="A2" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="n">
-        <v>41905</v>
-      </c>
-      <c r="C2" s="11" t="n">
+      <c r="B2" s="14" t="n">
+        <v>41898</v>
+      </c>
+      <c r="C2" s="13" t="n">
         <v>35</v>
       </c>
-      <c r="D2" s="11" t="n">
+      <c r="D2" s="13" t="n">
         <f aca="false">SUMIF(_cS, A2, _cHE)</f>
-        <v>21</v>
-      </c>
-      <c r="E2" s="13" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="E2" s="15" t="n">
         <f aca="false">SUMIF(_cS, A2, _cPIDHE)</f>
-        <v>0.175</v>
-      </c>
-      <c r="F2" s="13" t="inlineStr">
+        <v>0.0692771084337349</v>
+      </c>
+      <c r="F2" s="15" t="inlineStr">
         <f aca="false">E2</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G2" s="13" t="n">
+      <c r="G2" s="15" t="n">
         <f aca="false">SUMIF(_cS, A2, _cPIDHO)</f>
-        <v>0.0291666666666667</v>
-      </c>
-      <c r="H2" s="13" t="inlineStr">
+        <v>0.00903614457831325</v>
+      </c>
+      <c r="H2" s="15" t="inlineStr">
         <f aca="false">G2</f>
         <is>
           <t/>
@@ -1867,37 +2220,37 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="3">
-      <c r="A3" s="11" t="n">
+      <c r="A3" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="inlineStr">
+      <c r="B3" s="14" t="inlineStr">
         <f aca="false">B2+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C3" s="11" t="n">
+      <c r="C3" s="13" t="n">
         <v>35</v>
       </c>
-      <c r="D3" s="11" t="n">
+      <c r="D3" s="13" t="n">
         <f aca="false">SUMIF(_cS, A3, _cHE)</f>
-        <v>27</v>
-      </c>
-      <c r="E3" s="13" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="E3" s="15" t="n">
         <f aca="false">SUMIF(_cS, A3, _cPIDHE)</f>
-        <v>0.225</v>
-      </c>
-      <c r="F3" s="13" t="inlineStr">
+        <v>0.105421686746988</v>
+      </c>
+      <c r="F3" s="15" t="inlineStr">
         <f aca="false">E3+F2</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G3" s="13" t="n">
+      <c r="G3" s="15" t="n">
         <f aca="false">SUMIF(_cS, A3, _cPIDHO)</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="13" t="inlineStr">
+        <v>0.0120481927710843</v>
+      </c>
+      <c r="H3" s="15" t="inlineStr">
         <f aca="false">G3+H2</f>
         <is>
           <t/>
@@ -1905,37 +2258,37 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="4">
-      <c r="A4" s="11" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="12" t="inlineStr">
+      <c r="A4" s="13" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="14" t="inlineStr">
         <f aca="false">B3+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C4" s="11" t="n">
+      <c r="C4" s="13" t="n">
         <v>35</v>
       </c>
-      <c r="D4" s="11" t="n">
+      <c r="D4" s="13" t="n">
         <f aca="false">SUMIF(_cS, A4, _cHE)</f>
-        <v>34</v>
-      </c>
-      <c r="E4" s="13" t="n">
+        <v>39</v>
+      </c>
+      <c r="E4" s="15" t="n">
         <f aca="false">SUMIF(_cS, A4, _cPIDHE)</f>
-        <v>0.283333333333333</v>
-      </c>
-      <c r="F4" s="13" t="inlineStr">
+        <v>0.234939759036145</v>
+      </c>
+      <c r="F4" s="15" t="inlineStr">
         <f aca="false">E4+F3</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G4" s="13" t="n">
+      <c r="G4" s="15" t="n">
         <f aca="false">SUMIF(_cS, A4, _cPIDHO)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="13" t="inlineStr">
+      <c r="H4" s="15" t="inlineStr">
         <f aca="false">G4+H3</f>
         <is>
           <t/>
@@ -1943,37 +2296,37 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="5">
-      <c r="A5" s="11" t="n">
+      <c r="A5" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="inlineStr">
+      <c r="B5" s="14" t="inlineStr">
         <f aca="false">B4+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C5" s="11" t="n">
+      <c r="C5" s="13" t="n">
         <v>35</v>
       </c>
-      <c r="D5" s="11" t="n">
+      <c r="D5" s="13" t="n">
         <f aca="false">SUMIF(_cS, A5, _cHE)</f>
-        <v>27</v>
-      </c>
-      <c r="E5" s="13" t="n">
+        <v>34</v>
+      </c>
+      <c r="E5" s="15" t="n">
         <f aca="false">SUMIF(_cS, A5, _cPIDHE)</f>
-        <v>0.225</v>
-      </c>
-      <c r="F5" s="13" t="inlineStr">
+        <v>0.204819277108434</v>
+      </c>
+      <c r="F5" s="15" t="inlineStr">
         <f aca="false">E5+F4</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G5" s="13" t="n">
+      <c r="G5" s="15" t="n">
         <f aca="false">SUMIF(_cS, A5, _cPIDHO)</f>
         <v>0</v>
       </c>
-      <c r="H5" s="13" t="inlineStr">
+      <c r="H5" s="15" t="inlineStr">
         <f aca="false">G5+H4</f>
         <is>
           <t/>
@@ -1981,37 +2334,37 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="6">
-      <c r="A6" s="11" t="n">
+      <c r="A6" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="inlineStr">
+      <c r="B6" s="14" t="inlineStr">
         <f aca="false">B5+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C6" s="11" t="n">
+      <c r="C6" s="13" t="n">
         <v>35</v>
       </c>
-      <c r="D6" s="11" t="n">
+      <c r="D6" s="13" t="n">
         <f aca="false">SUMIF(_cS, A6, _cHE)</f>
-        <v>11</v>
-      </c>
-      <c r="E6" s="13" t="n">
+        <v>37</v>
+      </c>
+      <c r="E6" s="15" t="n">
         <f aca="false">SUMIF(_cS, A6, _cPIDHE)</f>
-        <v>0.0916666666666667</v>
-      </c>
-      <c r="F6" s="13" t="inlineStr">
+        <v>0.22289156626506</v>
+      </c>
+      <c r="F6" s="15" t="inlineStr">
         <f aca="false">E6+F5</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G6" s="13" t="n">
+      <c r="G6" s="15" t="n">
         <f aca="false">SUMIF(_cS, A6, _cPIDHO)</f>
         <v>0</v>
       </c>
-      <c r="H6" s="13" t="inlineStr">
+      <c r="H6" s="15" t="inlineStr">
         <f aca="false">G6+H5</f>
         <is>
           <t/>
@@ -2019,37 +2372,37 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="7">
-      <c r="A7" s="11" t="n">
+      <c r="A7" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="inlineStr">
+      <c r="B7" s="14" t="inlineStr">
         <f aca="false">B6+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C7" s="11" t="n">
+      <c r="C7" s="13" t="n">
         <v>35</v>
       </c>
-      <c r="D7" s="11" t="n">
+      <c r="D7" s="13" t="n">
         <f aca="false">SUMIF(_cS, A7, _cHE)</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="13" t="n">
+        <v>27</v>
+      </c>
+      <c r="E7" s="15" t="n">
         <f aca="false">SUMIF(_cS, A7, _cPIDHE)</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="13" t="inlineStr">
+        <v>0.162650602409639</v>
+      </c>
+      <c r="F7" s="15" t="inlineStr">
         <f aca="false">E7+F6</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G7" s="13" t="n">
+      <c r="G7" s="15" t="n">
         <f aca="false">SUMIF(_cS, A7, _cPIDHO)</f>
         <v>0</v>
       </c>
-      <c r="H7" s="13" t="inlineStr">
+      <c r="H7" s="15" t="inlineStr">
         <f aca="false">G7+H6</f>
         <is>
           <t/>
@@ -2057,37 +2410,37 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="8">
-      <c r="A8" s="11" t="n">
+      <c r="A8" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="12" t="inlineStr">
+      <c r="B8" s="14" t="inlineStr">
         <f aca="false">B7+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C8" s="11" t="n">
+      <c r="C8" s="13" t="n">
         <v>35</v>
       </c>
-      <c r="D8" s="11" t="n">
+      <c r="D8" s="13" t="n">
         <f aca="false">SUMIF(_cS, A8, _cHE)</f>
         <v>0</v>
       </c>
-      <c r="E8" s="13" t="n">
+      <c r="E8" s="15" t="n">
         <f aca="false">SUMIF(_cS, A8, _cPIDHE)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="13" t="inlineStr">
+      <c r="F8" s="15" t="inlineStr">
         <f aca="false">E8+F7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G8" s="13" t="n">
+      <c r="G8" s="15" t="n">
         <f aca="false">SUMIF(_cS, A8, _cPIDHO)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="13" t="inlineStr">
+      <c r="H8" s="15" t="inlineStr">
         <f aca="false">G8+H7</f>
         <is>
           <t/>
@@ -2095,37 +2448,37 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="9">
-      <c r="A9" s="11" t="n">
+      <c r="A9" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="12" t="inlineStr">
+      <c r="B9" s="14" t="inlineStr">
         <f aca="false">B8+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C9" s="11" t="n">
+      <c r="C9" s="13" t="n">
         <v>35</v>
       </c>
-      <c r="D9" s="11" t="n">
+      <c r="D9" s="13" t="n">
         <f aca="false">SUMIF(_cS, A9, _cHE)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="13" t="n">
+      <c r="E9" s="15" t="n">
         <f aca="false">SUMIF(_cS, A9, _cPIDHE)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="13" t="inlineStr">
+      <c r="F9" s="15" t="inlineStr">
         <f aca="false">E9+F8</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G9" s="13" t="n">
+      <c r="G9" s="15" t="n">
         <f aca="false">SUMIF(_cS, A9, _cPIDHO)</f>
         <v>0</v>
       </c>
-      <c r="H9" s="13" t="inlineStr">
+      <c r="H9" s="15" t="inlineStr">
         <f aca="false">G9+H8</f>
         <is>
           <t/>
@@ -2133,37 +2486,37 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="10">
-      <c r="A10" s="11" t="n">
+      <c r="A10" s="13" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="12" t="inlineStr">
+      <c r="B10" s="14" t="inlineStr">
         <f aca="false">B9+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C10" s="11" t="n">
+      <c r="C10" s="13" t="n">
         <v>35</v>
       </c>
-      <c r="D10" s="11" t="n">
+      <c r="D10" s="13" t="n">
         <f aca="false">SUMIF(_cS, A10, _cHE)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="13" t="n">
+      <c r="E10" s="15" t="n">
         <f aca="false">SUMIF(_cS, A10, _cPIDHE)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="13" t="inlineStr">
+      <c r="F10" s="15" t="inlineStr">
         <f aca="false">E10+F9</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G10" s="13" t="n">
+      <c r="G10" s="15" t="n">
         <f aca="false">SUMIF(_cS, A10, _cPIDHO)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="13" t="inlineStr">
+      <c r="H10" s="15" t="inlineStr">
         <f aca="false">G10+H9</f>
         <is>
           <t/>
@@ -2171,37 +2524,37 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="11">
-      <c r="A11" s="11" t="n">
+      <c r="A11" s="13" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="12" t="inlineStr">
+      <c r="B11" s="14" t="inlineStr">
         <f aca="false">B10+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C11" s="11" t="n">
+      <c r="C11" s="13" t="n">
         <v>35</v>
       </c>
-      <c r="D11" s="11" t="n">
+      <c r="D11" s="13" t="n">
         <f aca="false">SUMIF(_cS, A11, _cHE)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="13" t="n">
+      <c r="E11" s="15" t="n">
         <f aca="false">SUMIF(_cS, A11, _cPIDHE)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="13" t="inlineStr">
+      <c r="F11" s="15" t="inlineStr">
         <f aca="false">E11+F10</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G11" s="13" t="n">
+      <c r="G11" s="15" t="n">
         <f aca="false">SUMIF(_cS, A11, _cPIDHO)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="13" t="inlineStr">
+      <c r="H11" s="15" t="inlineStr">
         <f aca="false">G11+H10</f>
         <is>
           <t/>
@@ -2209,38 +2562,76 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="12">
-      <c r="A12" s="11" t="n">
+      <c r="A12" s="13" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="12" t="inlineStr">
+      <c r="B12" s="14" t="inlineStr">
         <f aca="false">B11+7</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="C12" s="11" t="n">
+      <c r="C12" s="13" t="n">
         <v>35</v>
       </c>
-      <c r="D12" s="11" t="n">
+      <c r="D12" s="13" t="n">
         <f aca="false">SUMIF(_cS, A12, _cHE)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="13" t="n">
+      <c r="E12" s="15" t="n">
         <f aca="false">SUMIF(_cS, A12, _cPIDHE)</f>
         <v>0</v>
       </c>
-      <c r="F12" s="13" t="inlineStr">
+      <c r="F12" s="15" t="inlineStr">
         <f aca="false">E12+F11</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="G12" s="13" t="n">
+      <c r="G12" s="15" t="n">
         <f aca="false">SUMIF(_cS, A12, _cPIDHO)</f>
         <v>0</v>
       </c>
-      <c r="H12" s="13" t="inlineStr">
+      <c r="H12" s="15" t="inlineStr">
         <f aca="false">G12+H11</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="13">
+      <c r="A13" s="13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="16" t="inlineStr">
+        <f aca="false">B12+7</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C13" s="13" t="n">
+        <v>35</v>
+      </c>
+      <c r="D13" s="13" t="n">
+        <f aca="false">SUMIF(_cS, A13, _cHE)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="15" t="n">
+        <f aca="false">SUMIF(_cS, A13, _cPIDHE)</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="15" t="inlineStr">
+        <f aca="false">E13+F12</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="G13" s="15" t="n">
+        <f aca="false">SUMIF(_cS, A13, _cPIDHO)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="15" t="inlineStr">
+        <f aca="false">G13+H12</f>
         <is>
           <t/>
         </is>
@@ -2256,4 +2647,667 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="1:21"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="I21" activeCellId="0" pane="topLeft" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="3.01960784313725"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="37.3372549019608"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="12.5529411764706"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="17.3411764705882"/>
+    <col collapsed="false" hidden="true" max="6" min="5" style="6" width="0"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="17" width="12.8588235294118"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="12.8588235294118"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="12.8666666666667"/>
+    <col collapsed="false" hidden="true" max="13" min="13" style="2" width="0"/>
+    <col collapsed="false" hidden="false" max="1022" min="14" style="2" width="8.41960784313726"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.41960784313726"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1" s="12">
+      <c r="A1" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="9"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="2" s="12">
+      <c r="A2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="3">
+      <c r="A3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="17" t="n">
+        <v>41899</v>
+      </c>
+      <c r="H3" s="17" t="n">
+        <v>41899</v>
+      </c>
+      <c r="I3" s="17" t="n">
+        <v>41899</v>
+      </c>
+      <c r="J3" s="17" t="n">
+        <v>41899</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <f aca="false">15/60</f>
+        <v>0.25</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="4">
+      <c r="A4" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="17" t="n">
+        <v>41899</v>
+      </c>
+      <c r="H4" s="17" t="n">
+        <v>41899</v>
+      </c>
+      <c r="I4" s="17" t="n">
+        <v>41899</v>
+      </c>
+      <c r="J4" s="17" t="n">
+        <v>41899</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L4" s="2" t="n">
+        <f aca="false">40/60</f>
+        <v>0.666666666666667</v>
+      </c>
+      <c r="M4" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="5">
+      <c r="A5" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="17" t="n">
+        <v>41899</v>
+      </c>
+      <c r="H5" s="17" t="n">
+        <v>41899</v>
+      </c>
+      <c r="I5" s="17" t="n">
+        <v>41899</v>
+      </c>
+      <c r="J5" s="17" t="n">
+        <v>41899</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <f aca="false">25/60</f>
+        <v>0.416666666666667</v>
+      </c>
+      <c r="M5" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="6">
+      <c r="A6" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G6" s="17" t="n">
+        <v>41900</v>
+      </c>
+      <c r="I6" s="17" t="n">
+        <v>41900</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="7">
+      <c r="A7" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="17" t="n">
+        <v>41901</v>
+      </c>
+      <c r="H7" s="17" t="n">
+        <v>41905</v>
+      </c>
+      <c r="I7" s="17" t="n">
+        <v>41901</v>
+      </c>
+      <c r="J7" s="17" t="n">
+        <v>41905</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <f aca="false">35/60</f>
+        <v>0.583333333333333</v>
+      </c>
+      <c r="M7" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="8">
+      <c r="A8" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="17" t="n">
+        <v>41902</v>
+      </c>
+      <c r="H8" s="17" t="n">
+        <v>41910</v>
+      </c>
+      <c r="I8" s="17" t="n">
+        <v>41902</v>
+      </c>
+      <c r="J8" s="17" t="n">
+        <v>41911</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="L8" s="2" t="n">
+        <f aca="false">(45+72)/60</f>
+        <v>1.95</v>
+      </c>
+      <c r="M8" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="9">
+      <c r="A9" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="17" t="n">
+        <v>41902</v>
+      </c>
+      <c r="H9" s="17" t="n">
+        <v>41910</v>
+      </c>
+      <c r="I9" s="17" t="n">
+        <v>41902</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="M9" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="10">
+      <c r="A10" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="17" t="n">
+        <v>41903</v>
+      </c>
+      <c r="I10" s="17" t="n">
+        <v>41903</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="M10" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="11">
+      <c r="A11" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="17" t="n">
+        <v>41903</v>
+      </c>
+      <c r="I11" s="17" t="n">
+        <v>41903</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M11" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="12">
+      <c r="A12" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="17" t="n">
+        <v>41905</v>
+      </c>
+      <c r="I12" s="17" t="n">
+        <v>41905</v>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="M12" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="13">
+      <c r="A13" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="17" t="n">
+        <v>41906</v>
+      </c>
+      <c r="I13" s="17" t="n">
+        <v>41906</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="M13" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="14">
+      <c r="A14" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G14" s="17" t="n">
+        <v>41907</v>
+      </c>
+      <c r="I14" s="17" t="n">
+        <v>41907</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="M14" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="15">
+      <c r="A15" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="17" t="n">
+        <v>41908</v>
+      </c>
+      <c r="I15" s="17" t="n">
+        <v>41908</v>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="M15" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="16">
+      <c r="A16" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="17" t="n">
+        <v>41910</v>
+      </c>
+      <c r="I16" s="17" t="n">
+        <v>41910</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M16" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="17">
+      <c r="A17" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="17" t="n">
+        <v>41912</v>
+      </c>
+      <c r="I17" s="17" t="n">
+        <v>41912</v>
+      </c>
+      <c r="K17" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="M17" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="18">
+      <c r="A18" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="17" t="n">
+        <v>41913</v>
+      </c>
+      <c r="I18" s="17" t="n">
+        <v>41913</v>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="M18" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="19">
+      <c r="A19" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="17" t="n">
+        <v>41913</v>
+      </c>
+      <c r="I19" s="17" t="n">
+        <v>41913</v>
+      </c>
+      <c r="K19" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="M19" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="20">
+      <c r="A20" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="17" t="n">
+        <v>41913</v>
+      </c>
+      <c r="I20" s="17" t="n">
+        <v>41913</v>
+      </c>
+      <c r="K20" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M20" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="21">
+      <c r="A21" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G21" s="17" t="n">
+        <v>41915</v>
+      </c>
+      <c r="I21" s="17" t="n">
+        <v>41915</v>
+      </c>
+      <c r="K21" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="M21" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:L1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
On branch master Changes to be committed: 	modified:   planes.xlsx
</commit_message>
<xml_diff>
--- a/planes.xlsx
+++ b/planes.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="142">
   <si>
     <t>Total de Horas Disponibles</t>
   </si>
@@ -87,7 +87,7 @@
     <t>Agenda para la reunion #1 con el cliente.</t>
   </si>
   <si>
-    <t>Experimiento RedMine #1</t>
+    <t>Experimiento RedMine #1; Instalar y configurar la última versión de RedMine.</t>
   </si>
   <si>
     <t>Reunión #1 con el cliente.</t>
@@ -445,6 +445,15 @@
   </si>
   <si>
     <t>HVR; AA</t>
+  </si>
+  <si>
+    <t>JGR; HVR; GW</t>
+  </si>
+  <si>
+    <t>HVR; AA;</t>
+  </si>
+  <si>
+    <t>JGR; JV; GW</t>
   </si>
 </sst>
 </file>
@@ -564,7 +573,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
@@ -599,7 +608,6 @@
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="167" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="167" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="168" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
     </xf>
@@ -678,7 +686,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -907,11 +915,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="92389958"/>
-        <c:axId val="94794816"/>
+        <c:axId val="82999205"/>
+        <c:axId val="5123968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92389958"/>
+        <c:axId val="82999205"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -919,7 +927,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94794816"/>
+        <c:crossAx val="5123968"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -933,7 +941,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94794816"/>
+        <c:axId val="5123968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -950,7 +958,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92389958"/>
+        <c:crossAx val="82999205"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -987,15 +995,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>167400</xdr:colOff>
+      <xdr:colOff>194400</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>34920</xdr:rowOff>
+      <xdr:rowOff>25920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>93960</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>153720</xdr:rowOff>
+      <xdr:colOff>120600</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>6120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1003,8 +1011,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9179280" y="34920"/>
-        <a:ext cx="8120520" cy="3219480"/>
+        <a:off x="9211320" y="25920"/>
+        <a:ext cx="8125200" cy="2556720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1025,12 +1033,12 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C9" activeCellId="1" pane="topLeft" sqref="I21 C9"/>
+      <selection activeCell="C9" activeCellId="0" pane="topLeft" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.8117647058824"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="2" width="8.41960784313726"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.8313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="2" width="8.42352941176471"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
@@ -1091,22 +1099,22 @@
   </sheetPr>
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H20" activeCellId="1" pane="topLeft" sqref="I21 H20"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A10" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D3" activeCellId="0" pane="topLeft" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="5" width="3.01960784313725"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="37.3372549019608"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="12.5529411764706"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="27.8352941176471"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="27.8470588235294"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="12.8588235294118"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="12.8666666666667"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="12.8666666666667"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="4" width="12.8666666666667"/>
-    <col collapsed="false" hidden="false" max="1022" min="10" style="2" width="8.41960784313726"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.41960784313726"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="37.3607843137255"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="12.5647058823529"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="27.8549019607843"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="27.8666666666667"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="12.8666666666667"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="12.8745098039216"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="12.8745098039216"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="4" width="12.8745098039216"/>
+    <col collapsed="false" hidden="false" max="1022" min="10" style="2" width="8.42352941176471"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.42352941176471"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="1" s="12">
@@ -1219,7 +1227,7 @@
         </is>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="5">
       <c r="A5" s="5" t="n">
         <v>4</v>
       </c>
@@ -2150,12 +2158,12 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F7" activeCellId="1" pane="topLeft" sqref="I21 F7"/>
+      <selection activeCell="A11" activeCellId="0" pane="topLeft" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="2" width="11.6392156862745"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="2" width="10.5843137254902"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="2" width="11.6470588235294"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="2" width="10.5921568627451"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="51.65" outlineLevel="0" r="1" s="12">
@@ -2603,7 +2611,7 @@
       <c r="A13" s="13" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="16" t="inlineStr">
+      <c r="B13" s="14" t="inlineStr">
         <f aca="false">B12+7</f>
         <is>
           <t/>
@@ -2654,24 +2662,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="I21" activeCellId="0" pane="topLeft" sqref="I21"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D20" activeCellId="0" pane="topLeft" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="5" width="3.01960784313725"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="37.3372549019608"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="12.5529411764706"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="17.3411764705882"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="37.3607843137255"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="12.5647058823529"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="17.356862745098"/>
     <col collapsed="false" hidden="true" max="6" min="5" style="6" width="0"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="17" width="12.8588235294118"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="12.8588235294118"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="12.8666666666667"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="16" width="12.8666666666667"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="12.8666666666667"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="12.8745098039216"/>
     <col collapsed="false" hidden="true" max="13" min="13" style="2" width="0"/>
-    <col collapsed="false" hidden="false" max="1022" min="14" style="2" width="8.41960784313726"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.41960784313726"/>
+    <col collapsed="false" hidden="false" max="1022" min="14" style="2" width="8.42352941176471"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.42352941176471"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1" s="12">
@@ -2690,8 +2698,6 @@
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="9"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="2" s="12">
       <c r="A2" s="8" t="s">
@@ -2712,16 +2718,16 @@
       <c r="F2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>134</v>
       </c>
       <c r="K2" s="9" t="s">
@@ -2733,10 +2739,8 @@
       <c r="M2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AMI2" s="0"/>
-      <c r="AMJ2" s="0"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="3">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="51.65" outlineLevel="0" r="3">
       <c r="A3" s="5" t="n">
         <v>1</v>
       </c>
@@ -2749,16 +2753,16 @@
       <c r="F3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="17" t="n">
+      <c r="G3" s="16" t="n">
         <v>41899</v>
       </c>
-      <c r="H3" s="17" t="n">
+      <c r="H3" s="16" t="n">
         <v>41899</v>
       </c>
-      <c r="I3" s="17" t="n">
+      <c r="I3" s="16" t="n">
         <v>41899</v>
       </c>
-      <c r="J3" s="17" t="n">
+      <c r="J3" s="16" t="n">
         <v>41899</v>
       </c>
       <c r="K3" s="2" t="n">
@@ -2772,7 +2776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="51.65" outlineLevel="0" r="4">
       <c r="A4" s="5" t="n">
         <v>2</v>
       </c>
@@ -2785,16 +2789,16 @@
       <c r="F4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="17" t="n">
+      <c r="G4" s="16" t="n">
         <v>41899</v>
       </c>
-      <c r="H4" s="17" t="n">
+      <c r="H4" s="16" t="n">
         <v>41899</v>
       </c>
-      <c r="I4" s="17" t="n">
+      <c r="I4" s="16" t="n">
         <v>41899</v>
       </c>
-      <c r="J4" s="17" t="n">
+      <c r="J4" s="16" t="n">
         <v>41899</v>
       </c>
       <c r="K4" s="2" t="n">
@@ -2808,7 +2812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="51.65" outlineLevel="0" r="5">
       <c r="A5" s="5" t="n">
         <v>3</v>
       </c>
@@ -2821,16 +2825,16 @@
       <c r="F5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="17" t="n">
+      <c r="G5" s="16" t="n">
         <v>41899</v>
       </c>
-      <c r="H5" s="17" t="n">
+      <c r="H5" s="16" t="n">
         <v>41899</v>
       </c>
-      <c r="I5" s="17" t="n">
+      <c r="I5" s="16" t="n">
         <v>41899</v>
       </c>
-      <c r="J5" s="17" t="n">
+      <c r="J5" s="16" t="n">
         <v>41899</v>
       </c>
       <c r="K5" s="2" t="n">
@@ -2844,7 +2848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="6">
       <c r="A6" s="5" t="n">
         <v>4</v>
       </c>
@@ -2854,10 +2858,10 @@
       <c r="D6" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="G6" s="17" t="n">
+      <c r="G6" s="16" t="n">
         <v>41900</v>
       </c>
-      <c r="I6" s="17" t="n">
+      <c r="I6" s="16" t="n">
         <v>41900</v>
       </c>
       <c r="K6" s="2" t="n">
@@ -2867,7 +2871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="51.65" outlineLevel="0" r="7">
       <c r="A7" s="5" t="n">
         <v>5</v>
       </c>
@@ -2883,16 +2887,16 @@
       <c r="F7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="17" t="n">
+      <c r="G7" s="16" t="n">
         <v>41901</v>
       </c>
-      <c r="H7" s="17" t="n">
+      <c r="H7" s="16" t="n">
         <v>41905</v>
       </c>
-      <c r="I7" s="17" t="n">
+      <c r="I7" s="16" t="n">
         <v>41901</v>
       </c>
-      <c r="J7" s="17" t="n">
+      <c r="J7" s="16" t="n">
         <v>41905</v>
       </c>
       <c r="K7" s="2" t="n">
@@ -2906,7 +2910,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="64.15" outlineLevel="0" r="8">
       <c r="A8" s="5" t="n">
         <v>6</v>
       </c>
@@ -2919,16 +2923,16 @@
       <c r="F8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="17" t="n">
+      <c r="G8" s="16" t="n">
         <v>41902</v>
       </c>
-      <c r="H8" s="17" t="n">
+      <c r="H8" s="16" t="n">
         <v>41910</v>
       </c>
-      <c r="I8" s="17" t="n">
+      <c r="I8" s="16" t="n">
         <v>41902</v>
       </c>
-      <c r="J8" s="17" t="n">
+      <c r="J8" s="16" t="n">
         <v>41911</v>
       </c>
       <c r="K8" s="2" t="n">
@@ -2942,7 +2946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="76.65" outlineLevel="0" r="9">
       <c r="A9" s="5" t="n">
         <v>7</v>
       </c>
@@ -2958,13 +2962,13 @@
       <c r="F9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="17" t="n">
+      <c r="G9" s="16" t="n">
         <v>41902</v>
       </c>
-      <c r="H9" s="17" t="n">
+      <c r="H9" s="16" t="n">
         <v>41910</v>
       </c>
-      <c r="I9" s="17" t="n">
+      <c r="I9" s="16" t="n">
         <v>41902</v>
       </c>
       <c r="K9" s="2" t="n">
@@ -2974,7 +2978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="76.65" outlineLevel="0" r="10">
       <c r="A10" s="5" t="n">
         <v>8</v>
       </c>
@@ -2984,13 +2988,16 @@
       <c r="C10" s="7" t="s">
         <v>29</v>
       </c>
+      <c r="D10" s="6" t="s">
+        <v>139</v>
+      </c>
       <c r="F10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="17" t="n">
+      <c r="G10" s="16" t="n">
         <v>41903</v>
       </c>
-      <c r="I10" s="17" t="n">
+      <c r="I10" s="16" t="n">
         <v>41903</v>
       </c>
       <c r="K10" s="2" t="n">
@@ -3000,7 +3007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="51.65" outlineLevel="0" r="11">
       <c r="A11" s="5" t="n">
         <v>9</v>
       </c>
@@ -3016,10 +3023,10 @@
       <c r="F11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="17" t="n">
+      <c r="G11" s="16" t="n">
         <v>41903</v>
       </c>
-      <c r="I11" s="17" t="n">
+      <c r="I11" s="16" t="n">
         <v>41903</v>
       </c>
       <c r="K11" s="2" t="n">
@@ -3029,7 +3036,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="51.65" outlineLevel="0" r="12">
       <c r="A12" s="5" t="n">
         <v>10</v>
       </c>
@@ -3039,13 +3046,16 @@
       <c r="C12" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="D12" s="6" t="s">
+        <v>140</v>
+      </c>
       <c r="F12" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="17" t="n">
+      <c r="G12" s="16" t="n">
         <v>41905</v>
       </c>
-      <c r="I12" s="17" t="n">
+      <c r="I12" s="16" t="n">
         <v>41905</v>
       </c>
       <c r="K12" s="2" t="n">
@@ -3055,7 +3065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="76.65" outlineLevel="0" r="13">
       <c r="A13" s="5" t="n">
         <v>11</v>
       </c>
@@ -3071,10 +3081,10 @@
       <c r="F13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="17" t="n">
+      <c r="G13" s="16" t="n">
         <v>41906</v>
       </c>
-      <c r="I13" s="17" t="n">
+      <c r="I13" s="16" t="n">
         <v>41906</v>
       </c>
       <c r="K13" s="2" t="n">
@@ -3097,10 +3107,10 @@
       <c r="D14" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="G14" s="17" t="n">
+      <c r="G14" s="16" t="n">
         <v>41907</v>
       </c>
-      <c r="I14" s="17" t="n">
+      <c r="I14" s="16" t="n">
         <v>41907</v>
       </c>
       <c r="K14" s="2" t="n">
@@ -3110,7 +3120,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="76.65" outlineLevel="0" r="15">
       <c r="A15" s="5" t="n">
         <v>13</v>
       </c>
@@ -3120,13 +3130,16 @@
       <c r="C15" s="7" t="s">
         <v>43</v>
       </c>
+      <c r="D15" s="6" t="s">
+        <v>141</v>
+      </c>
       <c r="F15" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="17" t="n">
+      <c r="G15" s="16" t="n">
         <v>41908</v>
       </c>
-      <c r="I15" s="17" t="n">
+      <c r="I15" s="16" t="n">
         <v>41908</v>
       </c>
       <c r="K15" s="2" t="n">
@@ -3136,7 +3149,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="51.65" outlineLevel="0" r="16">
       <c r="A16" s="5" t="n">
         <v>14</v>
       </c>
@@ -3152,10 +3165,10 @@
       <c r="F16" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="17" t="n">
+      <c r="G16" s="16" t="n">
         <v>41910</v>
       </c>
-      <c r="I16" s="17" t="n">
+      <c r="I16" s="16" t="n">
         <v>41910</v>
       </c>
       <c r="K16" s="2" t="n">
@@ -3165,7 +3178,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="51.65" outlineLevel="0" r="17">
       <c r="A17" s="5" t="n">
         <v>15</v>
       </c>
@@ -3178,10 +3191,10 @@
       <c r="F17" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G17" s="17" t="n">
+      <c r="G17" s="16" t="n">
         <v>41912</v>
       </c>
-      <c r="I17" s="17" t="n">
+      <c r="I17" s="16" t="n">
         <v>41912</v>
       </c>
       <c r="K17" s="2" t="n">
@@ -3191,7 +3204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="76.65" outlineLevel="0" r="18">
       <c r="A18" s="5" t="n">
         <v>16</v>
       </c>
@@ -3201,13 +3214,16 @@
       <c r="C18" s="7" t="s">
         <v>52</v>
       </c>
+      <c r="D18" s="6" t="s">
+        <v>137</v>
+      </c>
       <c r="F18" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G18" s="17" t="n">
+      <c r="G18" s="16" t="n">
         <v>41913</v>
       </c>
-      <c r="I18" s="17" t="n">
+      <c r="I18" s="16" t="n">
         <v>41913</v>
       </c>
       <c r="K18" s="2" t="n">
@@ -3217,7 +3233,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="76.65" outlineLevel="0" r="19">
       <c r="A19" s="5" t="n">
         <v>17</v>
       </c>
@@ -3227,13 +3243,16 @@
       <c r="C19" s="7" t="s">
         <v>55</v>
       </c>
+      <c r="D19" s="6" t="s">
+        <v>141</v>
+      </c>
       <c r="F19" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G19" s="17" t="n">
+      <c r="G19" s="16" t="n">
         <v>41913</v>
       </c>
-      <c r="I19" s="17" t="n">
+      <c r="I19" s="16" t="n">
         <v>41913</v>
       </c>
       <c r="K19" s="2" t="n">
@@ -3243,7 +3262,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="51.65" outlineLevel="0" r="20">
       <c r="A20" s="5" t="n">
         <v>18</v>
       </c>
@@ -3259,10 +3278,10 @@
       <c r="F20" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G20" s="17" t="n">
+      <c r="G20" s="16" t="n">
         <v>41913</v>
       </c>
-      <c r="I20" s="17" t="n">
+      <c r="I20" s="16" t="n">
         <v>41913</v>
       </c>
       <c r="K20" s="2" t="n">
@@ -3272,7 +3291,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="51.65" outlineLevel="0" r="21">
       <c r="A21" s="5" t="n">
         <v>19</v>
       </c>
@@ -3285,10 +3304,10 @@
       <c r="F21" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="G21" s="17" t="n">
+      <c r="G21" s="16" t="n">
         <v>41915</v>
       </c>
-      <c r="I21" s="17" t="n">
+      <c r="I21" s="16" t="n">
         <v>41915</v>
       </c>
       <c r="K21" s="2" t="n">

</xml_diff>

<commit_message>
Formas de Planes y Tares Individuales Ciclo #1 Agrege las formas de los planes y tareas individuales para el ciclo 1. Así como también, la agenda de la reunión #1, y la modificación de mi log diario.
</commit_message>
<xml_diff>
--- a/planes.xlsx
+++ b/planes.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="3" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="456" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="456" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Totales" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Proyecto" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Recursos" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Ciclo1" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="TEAMTASK1" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="_cHE" vbProcedure="false">Proyecto!$F$2:$F$1048576</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="145">
   <si>
     <t>Total de Horas Disponibles</t>
   </si>
@@ -417,7 +418,7 @@
     <t>Porcentaje de las Ganacias Obtenidas</t>
   </si>
   <si>
-    <t>3 Semanas; 09/16/2014-10/06/2014</t>
+    <t>4 Semanas; 09/16/2014-10/06/2014</t>
   </si>
   <si>
     <t>Asignado a</t>
@@ -454,6 +455,15 @@
   </si>
   <si>
     <t>JGR; JV; GW</t>
+  </si>
+  <si>
+    <t># de Ingenieros</t>
+  </si>
+  <si>
+    <t>Estimado</t>
+  </si>
+  <si>
+    <t>Actual</t>
   </si>
 </sst>
 </file>
@@ -686,7 +696,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -915,11 +925,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="82999205"/>
-        <c:axId val="5123968"/>
+        <c:axId val="48334944"/>
+        <c:axId val="89466597"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82999205"/>
+        <c:axId val="48334944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -927,7 +937,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="5123968"/>
+        <c:crossAx val="89466597"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -941,7 +951,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="5123968"/>
+        <c:axId val="89466597"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -958,7 +968,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82999205"/>
+        <c:crossAx val="48334944"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -995,15 +1005,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>194400</xdr:colOff>
+      <xdr:colOff>126000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>25920</xdr:rowOff>
+      <xdr:rowOff>43560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>120600</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
+      <xdr:colOff>51480</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1011,8 +1021,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9211320" y="25920"/>
-        <a:ext cx="8125200" cy="2556720"/>
+        <a:off x="9153000" y="43560"/>
+        <a:ext cx="8134920" cy="2883960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1037,8 +1047,8 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.8313725490196"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="2" width="8.42352941176471"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.8705882352941"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="2" width="8.43921568627451"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
@@ -1099,22 +1109,22 @@
   </sheetPr>
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A10" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D3" activeCellId="0" pane="topLeft" sqref="D3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D4" activeCellId="0" pane="topLeft" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="5" width="3.01960784313725"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="37.3607843137255"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="12.5647058823529"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="27.8549019607843"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="27.8666666666667"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="12.8666666666667"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="12.8745098039216"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="12.8745098039216"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="4" width="12.8745098039216"/>
-    <col collapsed="false" hidden="false" max="1022" min="10" style="2" width="8.42352941176471"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.42352941176471"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="37.4156862745098"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="8.4"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="27.8941176470588"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="27.9058823529412"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="12.878431372549"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="12.8862745098039"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="12.8862745098039"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="4" width="12.8862745098039"/>
+    <col collapsed="false" hidden="false" max="1022" min="10" style="2" width="8.43921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.43921568627451"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="1" s="12">
@@ -2158,12 +2168,12 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A11" activeCellId="0" pane="topLeft" sqref="A11"/>
+      <selection activeCell="H23" activeCellId="0" pane="topLeft" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="2" width="11.6470588235294"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="2" width="10.5921568627451"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="2" width="11.6588235294118"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="2" width="10.6039215686275"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="51.65" outlineLevel="0" r="1" s="12">
@@ -2664,22 +2674,22 @@
   </sheetPr>
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D20" activeCellId="0" pane="topLeft" sqref="D20"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="5" width="3.01960784313725"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="37.3607843137255"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="12.5647058823529"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="17.356862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="37.4156862745098"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="12.5803921568627"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="17.3803921568627"/>
     <col collapsed="false" hidden="true" max="6" min="5" style="6" width="0"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="16" width="12.8666666666667"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="12.8666666666667"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="12.8745098039216"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="16" width="12.878431372549"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="12.878431372549"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="12.8862745098039"/>
     <col collapsed="false" hidden="true" max="13" min="13" style="2" width="0"/>
-    <col collapsed="false" hidden="false" max="1022" min="14" style="2" width="8.42352941176471"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.42352941176471"/>
+    <col collapsed="false" hidden="false" max="1022" min="14" style="2" width="8.43921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.43921568627451"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1" s="12">
@@ -2768,10 +2778,6 @@
       <c r="K3" s="2" t="n">
         <v>0.5</v>
       </c>
-      <c r="L3" s="2" t="n">
-        <f aca="false">15/60</f>
-        <v>0.25</v>
-      </c>
       <c r="M3" s="2" t="n">
         <v>1</v>
       </c>
@@ -2804,10 +2810,6 @@
       <c r="K4" s="2" t="n">
         <v>0.5</v>
       </c>
-      <c r="L4" s="2" t="n">
-        <f aca="false">40/60</f>
-        <v>0.666666666666667</v>
-      </c>
       <c r="M4" s="2" t="n">
         <v>1</v>
       </c>
@@ -2839,10 +2841,6 @@
       </c>
       <c r="K5" s="2" t="n">
         <v>0.5</v>
-      </c>
-      <c r="L5" s="2" t="n">
-        <f aca="false">25/60</f>
-        <v>0.416666666666667</v>
       </c>
       <c r="M5" s="2" t="n">
         <v>1</v>
@@ -2902,10 +2900,6 @@
       <c r="K7" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L7" s="2" t="n">
-        <f aca="false">35/60</f>
-        <v>0.583333333333333</v>
-      </c>
       <c r="M7" s="2" t="n">
         <v>2</v>
       </c>
@@ -2938,10 +2932,6 @@
       <c r="K8" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="L8" s="2" t="n">
-        <f aca="false">(45+72)/60</f>
-        <v>1.95</v>
-      </c>
       <c r="M8" s="2" t="n">
         <v>2</v>
       </c>
@@ -3026,8 +3016,14 @@
       <c r="G11" s="16" t="n">
         <v>41903</v>
       </c>
+      <c r="H11" s="16" t="n">
+        <v>41913</v>
+      </c>
       <c r="I11" s="16" t="n">
         <v>41903</v>
+      </c>
+      <c r="J11" s="16" t="n">
+        <v>41913</v>
       </c>
       <c r="K11" s="2" t="n">
         <v>0.5</v>
@@ -3329,4 +3325,105 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="1:2"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D3" activeCellId="0" pane="topLeft" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="8.4"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="3.01960784313725"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="37.4156862745098"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="6" width="8.4"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="6" width="12.878431372549"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="16" width="12.878431372549"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="12.878431372549"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="16" width="12.878431372549"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="12.8862745098039"/>
+    <col collapsed="false" hidden="false" max="1021" min="13" style="2" width="8.43921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.43921568627451"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="14.95" outlineLevel="0" r="1" s="12">
+      <c r="A1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="9"/>
+      <c r="G1" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="2" s="12">
+      <c r="A2" s="9"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="AMJ2" s="0"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>